<commit_message>
Actualizo dashboard y reporte de inflación
</commit_message>
<xml_diff>
--- a/Proyecto inflacion_Power BI/Inflacion_Analisis_protecto_Power BI.xlsx
+++ b/Proyecto inflacion_Power BI/Inflacion_Analisis_protecto_Power BI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAE2152-4C75-43C9-B16E-B8F0F9FF926F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61CD5F3-C412-48B6-961C-8785B0AC55D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="245">
   <si>
     <t>Año</t>
   </si>
@@ -217,6 +217,546 @@
   </si>
   <si>
     <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Jan-2007</t>
+  </si>
+  <si>
+    <t>Feb-2007</t>
+  </si>
+  <si>
+    <t>Mar-2007</t>
+  </si>
+  <si>
+    <t>Apr-2007</t>
+  </si>
+  <si>
+    <t>May-2007</t>
+  </si>
+  <si>
+    <t>Jun-2007</t>
+  </si>
+  <si>
+    <t>Jul-2007</t>
+  </si>
+  <si>
+    <t>Aug-2007</t>
+  </si>
+  <si>
+    <t>Sep-2007</t>
+  </si>
+  <si>
+    <t>Oct-2007</t>
+  </si>
+  <si>
+    <t>Nov-2007</t>
+  </si>
+  <si>
+    <t>Dec-2007</t>
+  </si>
+  <si>
+    <t>Jan-2008</t>
+  </si>
+  <si>
+    <t>Feb-2008</t>
+  </si>
+  <si>
+    <t>Mar-2008</t>
+  </si>
+  <si>
+    <t>Apr-2008</t>
+  </si>
+  <si>
+    <t>May-2008</t>
+  </si>
+  <si>
+    <t>Jun-2008</t>
+  </si>
+  <si>
+    <t>Jul-2008</t>
+  </si>
+  <si>
+    <t>Aug-2008</t>
+  </si>
+  <si>
+    <t>Sep-2008</t>
+  </si>
+  <si>
+    <t>Oct-2008</t>
+  </si>
+  <si>
+    <t>Nov-2008</t>
+  </si>
+  <si>
+    <t>Dec-2008</t>
+  </si>
+  <si>
+    <t>Jan-2009</t>
+  </si>
+  <si>
+    <t>Feb-2009</t>
+  </si>
+  <si>
+    <t>Mar-2009</t>
+  </si>
+  <si>
+    <t>Apr-2009</t>
+  </si>
+  <si>
+    <t>May-2009</t>
+  </si>
+  <si>
+    <t>Jun-2009</t>
+  </si>
+  <si>
+    <t>Jul-2009</t>
+  </si>
+  <si>
+    <t>Aug-2009</t>
+  </si>
+  <si>
+    <t>Sep-2009</t>
+  </si>
+  <si>
+    <t>Oct-2009</t>
+  </si>
+  <si>
+    <t>Nov-2009</t>
+  </si>
+  <si>
+    <t>Dec-2009</t>
+  </si>
+  <si>
+    <t>Jan-2010</t>
+  </si>
+  <si>
+    <t>Feb-2010</t>
+  </si>
+  <si>
+    <t>Mar-2010</t>
+  </si>
+  <si>
+    <t>Apr-2010</t>
+  </si>
+  <si>
+    <t>May-2010</t>
+  </si>
+  <si>
+    <t>Jun-2010</t>
+  </si>
+  <si>
+    <t>Jul-2010</t>
+  </si>
+  <si>
+    <t>Aug-2010</t>
+  </si>
+  <si>
+    <t>Sep-2010</t>
+  </si>
+  <si>
+    <t>Oct-2010</t>
+  </si>
+  <si>
+    <t>Nov-2010</t>
+  </si>
+  <si>
+    <t>Dec-2010</t>
+  </si>
+  <si>
+    <t>Jan-2011</t>
+  </si>
+  <si>
+    <t>Feb-2011</t>
+  </si>
+  <si>
+    <t>Mar-2011</t>
+  </si>
+  <si>
+    <t>Apr-2011</t>
+  </si>
+  <si>
+    <t>May-2011</t>
+  </si>
+  <si>
+    <t>Jun-2011</t>
+  </si>
+  <si>
+    <t>Jul-2011</t>
+  </si>
+  <si>
+    <t>Aug-2011</t>
+  </si>
+  <si>
+    <t>Sep-2011</t>
+  </si>
+  <si>
+    <t>Oct-2011</t>
+  </si>
+  <si>
+    <t>Nov-2011</t>
+  </si>
+  <si>
+    <t>Dec-2011</t>
+  </si>
+  <si>
+    <t>Jan-2012</t>
+  </si>
+  <si>
+    <t>Feb-2012</t>
+  </si>
+  <si>
+    <t>Mar-2012</t>
+  </si>
+  <si>
+    <t>Apr-2012</t>
+  </si>
+  <si>
+    <t>May-2012</t>
+  </si>
+  <si>
+    <t>Jun-2012</t>
+  </si>
+  <si>
+    <t>Jul-2012</t>
+  </si>
+  <si>
+    <t>Aug-2012</t>
+  </si>
+  <si>
+    <t>Sep-2012</t>
+  </si>
+  <si>
+    <t>Oct-2012</t>
+  </si>
+  <si>
+    <t>Nov-2012</t>
+  </si>
+  <si>
+    <t>Dec-2012</t>
+  </si>
+  <si>
+    <t>Jan-2013</t>
+  </si>
+  <si>
+    <t>Feb-2013</t>
+  </si>
+  <si>
+    <t>Mar-2013</t>
+  </si>
+  <si>
+    <t>Apr-2013</t>
+  </si>
+  <si>
+    <t>May-2013</t>
+  </si>
+  <si>
+    <t>Jun-2013</t>
+  </si>
+  <si>
+    <t>Jul-2013</t>
+  </si>
+  <si>
+    <t>Aug-2013</t>
+  </si>
+  <si>
+    <t>Sep-2013</t>
+  </si>
+  <si>
+    <t>Oct-2013</t>
+  </si>
+  <si>
+    <t>Nov-2013</t>
+  </si>
+  <si>
+    <t>Dec-2013</t>
+  </si>
+  <si>
+    <t>Jan-2014</t>
+  </si>
+  <si>
+    <t>Feb-2014</t>
+  </si>
+  <si>
+    <t>Mar-2014</t>
+  </si>
+  <si>
+    <t>Apr-2014</t>
+  </si>
+  <si>
+    <t>May-2014</t>
+  </si>
+  <si>
+    <t>Jun-2014</t>
+  </si>
+  <si>
+    <t>Jul-2014</t>
+  </si>
+  <si>
+    <t>Aug-2014</t>
+  </si>
+  <si>
+    <t>Sep-2014</t>
+  </si>
+  <si>
+    <t>Oct-2014</t>
+  </si>
+  <si>
+    <t>Nov-2014</t>
+  </si>
+  <si>
+    <t>Dec-2014</t>
+  </si>
+  <si>
+    <t>Jan-2015</t>
+  </si>
+  <si>
+    <t>Feb-2015</t>
+  </si>
+  <si>
+    <t>Mar-2015</t>
+  </si>
+  <si>
+    <t>Apr-2015</t>
+  </si>
+  <si>
+    <t>May-2015</t>
+  </si>
+  <si>
+    <t>Jun-2015</t>
+  </si>
+  <si>
+    <t>Jul-2015</t>
+  </si>
+  <si>
+    <t>Aug-2015</t>
+  </si>
+  <si>
+    <t>Sep-2015</t>
+  </si>
+  <si>
+    <t>Oct-2015</t>
+  </si>
+  <si>
+    <t>Nov-2015</t>
+  </si>
+  <si>
+    <t>Dec-2015</t>
+  </si>
+  <si>
+    <t>Jan-2016</t>
+  </si>
+  <si>
+    <t>Feb-2016</t>
+  </si>
+  <si>
+    <t>Mar-2016</t>
+  </si>
+  <si>
+    <t>Apr-2016</t>
+  </si>
+  <si>
+    <t>May-2016</t>
+  </si>
+  <si>
+    <t>Jun-2016</t>
+  </si>
+  <si>
+    <t>Jul-2016</t>
+  </si>
+  <si>
+    <t>Aug-2016</t>
+  </si>
+  <si>
+    <t>Sep-2016</t>
+  </si>
+  <si>
+    <t>Oct-2016</t>
+  </si>
+  <si>
+    <t>Nov-2016</t>
+  </si>
+  <si>
+    <t>Dec-2016</t>
+  </si>
+  <si>
+    <t>Jan-2017</t>
+  </si>
+  <si>
+    <t>Feb-2017</t>
+  </si>
+  <si>
+    <t>Mar-2017</t>
+  </si>
+  <si>
+    <t>Apr-2017</t>
+  </si>
+  <si>
+    <t>May-2017</t>
+  </si>
+  <si>
+    <t>Jun-2017</t>
+  </si>
+  <si>
+    <t>Jul-2017</t>
+  </si>
+  <si>
+    <t>Aug-2017</t>
+  </si>
+  <si>
+    <t>Sep-2017</t>
+  </si>
+  <si>
+    <t>Oct-2017</t>
+  </si>
+  <si>
+    <t>Nov-2017</t>
+  </si>
+  <si>
+    <t>Dec-2017</t>
+  </si>
+  <si>
+    <t>Jan-2018</t>
+  </si>
+  <si>
+    <t>Feb-2018</t>
+  </si>
+  <si>
+    <t>Mar-2018</t>
+  </si>
+  <si>
+    <t>Apr-2018</t>
+  </si>
+  <si>
+    <t>May-2018</t>
+  </si>
+  <si>
+    <t>Jun-2018</t>
+  </si>
+  <si>
+    <t>Jul-2018</t>
+  </si>
+  <si>
+    <t>Aug-2018</t>
+  </si>
+  <si>
+    <t>Sep-2018</t>
+  </si>
+  <si>
+    <t>Oct-2018</t>
+  </si>
+  <si>
+    <t>Nov-2018</t>
+  </si>
+  <si>
+    <t>Dec-2018</t>
+  </si>
+  <si>
+    <t>Jan-2019</t>
+  </si>
+  <si>
+    <t>Feb-2019</t>
+  </si>
+  <si>
+    <t>Mar-2019</t>
+  </si>
+  <si>
+    <t>Apr-2019</t>
+  </si>
+  <si>
+    <t>May-2019</t>
+  </si>
+  <si>
+    <t>Jun-2019</t>
+  </si>
+  <si>
+    <t>Jul-2019</t>
+  </si>
+  <si>
+    <t>Aug-2019</t>
+  </si>
+  <si>
+    <t>Sep-2019</t>
+  </si>
+  <si>
+    <t>Oct-2019</t>
+  </si>
+  <si>
+    <t>Nov-2019</t>
+  </si>
+  <si>
+    <t>Dec-2019</t>
+  </si>
+  <si>
+    <t>Jan-2020</t>
+  </si>
+  <si>
+    <t>Feb-2020</t>
+  </si>
+  <si>
+    <t>Mar-2020</t>
+  </si>
+  <si>
+    <t>Apr-2020</t>
+  </si>
+  <si>
+    <t>May-2020</t>
+  </si>
+  <si>
+    <t>Jun-2020</t>
+  </si>
+  <si>
+    <t>Jul-2020</t>
+  </si>
+  <si>
+    <t>Aug-2020</t>
+  </si>
+  <si>
+    <t>Sep-2020</t>
+  </si>
+  <si>
+    <t>Oct-2020</t>
+  </si>
+  <si>
+    <t>Nov-2020</t>
+  </si>
+  <si>
+    <t>Dec-2020</t>
+  </si>
+  <si>
+    <t>Jan-2021</t>
+  </si>
+  <si>
+    <t>Feb-2021</t>
+  </si>
+  <si>
+    <t>Mar-2021</t>
+  </si>
+  <si>
+    <t>Apr-2021</t>
+  </si>
+  <si>
+    <t>May-2021</t>
+  </si>
+  <si>
+    <t>Jun-2021</t>
+  </si>
+  <si>
+    <t>Jul-2021</t>
+  </si>
+  <si>
+    <t>Aug-2021</t>
+  </si>
+  <si>
+    <t>Sep-2021</t>
+  </si>
+  <si>
+    <t>Oct-2021</t>
+  </si>
+  <si>
+    <t>Nov-2021</t>
+  </si>
+  <si>
+    <t>Dec-2021</t>
   </si>
 </sst>
 </file>
@@ -281,34 +821,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
@@ -352,16 +864,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color auto="1"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color auto="1"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -394,16 +906,44 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color auto="1"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -420,7 +960,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{694616B3-BA51-425F-B9AB-57FE4D8C2653}" name="inflacion_anual" displayName="inflacion_anual" ref="A1:B20" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{694616B3-BA51-425F-B9AB-57FE4D8C2653}" name="inflacion_anual" displayName="inflacion_anual" ref="A1:B20" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:B20" xr:uid="{694616B3-BA51-425F-B9AB-57FE4D8C2653}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1B673370-C446-4E18-B4E4-CB0688F63C36}" name="Año"/>
@@ -431,7 +971,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C955C9C2-6EDB-40B0-9459-1D0C8A5A93AC}" name="promedio_inflacion" displayName="promedio_inflacion" ref="A1:B13" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C955C9C2-6EDB-40B0-9459-1D0C8A5A93AC}" name="promedio_inflacion" displayName="promedio_inflacion" ref="A1:B13" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:B13" xr:uid="{C955C9C2-6EDB-40B0-9459-1D0C8A5A93AC}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6449138E-ED68-4EB5-BEC8-35BBCE37066A}" name="Mes nombre"/>
@@ -442,8 +982,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4DDF443-31D2-4C83-8DB2-F38082501F26}" name="inflacion_mensual" displayName="inflacion_mensual" ref="A1:B49" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="8">
-  <autoFilter ref="A1:B49" xr:uid="{C4DDF443-31D2-4C83-8DB2-F38082501F26}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4DDF443-31D2-4C83-8DB2-F38082501F26}" name="inflacion_mensual" displayName="inflacion_mensual" ref="A1:B229" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:B229" xr:uid="{C4DDF443-31D2-4C83-8DB2-F38082501F26}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A26CF429-1399-4BCA-97E4-E06661591C39}" name="Mes-Año"/>
     <tableColumn id="2" xr3:uid="{E0E998C1-EB7F-4C19-B1F2-FA5EAB3D52E7}" name="Inflacion mensual"/>
@@ -922,7 +1462,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,385 +1607,1825 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="B2">
-        <v>3.9</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B3">
-        <v>4.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B4">
-        <v>6.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B6">
-        <v>5.0999999999999996</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B7">
-        <v>5.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B8">
-        <v>7.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B10">
-        <v>6.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B11">
-        <v>6.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B12">
-        <v>4.9000000000000004</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B13">
-        <v>5.0999999999999996</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B15">
-        <v>6.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B16">
-        <v>7.7</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B17">
-        <v>8.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B18">
-        <v>7.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B20">
-        <v>6.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="B21">
-        <v>12.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B22">
-        <v>12.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="B23">
-        <v>8.3000000000000007</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="B24">
-        <v>12.8</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B25">
-        <v>25.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B26">
-        <v>20.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B27">
-        <v>13.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B29">
-        <v>8.8000000000000007</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="B30">
-        <v>4.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="B31">
-        <v>4.5999999999999996</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="B33">
-        <v>4.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="B34">
-        <v>3.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="B35">
-        <v>2.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="B36">
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="B37">
-        <v>2.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="B38">
-        <v>2.2000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="B39">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="B40">
-        <v>3.7</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B41">
-        <v>2.8</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="B42">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="B43">
-        <v>1.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="B44">
-        <v>1.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="B45">
-        <v>1.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="B46">
-        <v>2.1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="B47">
-        <v>2.2999999999999998</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="B48">
-        <v>2.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>134</v>
+      </c>
+      <c r="B71">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>138</v>
+      </c>
+      <c r="B75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>147</v>
+      </c>
+      <c r="B84">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>149</v>
+      </c>
+      <c r="B86">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>154</v>
+      </c>
+      <c r="B91">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>157</v>
+      </c>
+      <c r="B94">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>158</v>
+      </c>
+      <c r="B95">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>159</v>
+      </c>
+      <c r="B96">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>160</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>162</v>
+      </c>
+      <c r="B99">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>163</v>
+      </c>
+      <c r="B100">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>164</v>
+      </c>
+      <c r="B101">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>173</v>
+      </c>
+      <c r="B110">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>174</v>
+      </c>
+      <c r="B111">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>176</v>
+      </c>
+      <c r="B113">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>177</v>
+      </c>
+      <c r="B114">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>179</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>180</v>
+      </c>
+      <c r="B117">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>181</v>
+      </c>
+      <c r="B118">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>182</v>
+      </c>
+      <c r="B119">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>183</v>
+      </c>
+      <c r="B120">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>184</v>
+      </c>
+      <c r="B121">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>185</v>
+      </c>
+      <c r="B122">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>186</v>
+      </c>
+      <c r="B123">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>187</v>
+      </c>
+      <c r="B124">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>188</v>
+      </c>
+      <c r="B125">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>189</v>
+      </c>
+      <c r="B126">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>190</v>
+      </c>
+      <c r="B127">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>191</v>
+      </c>
+      <c r="B128">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>192</v>
+      </c>
+      <c r="B129">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>193</v>
+      </c>
+      <c r="B130">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>194</v>
+      </c>
+      <c r="B131">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>195</v>
+      </c>
+      <c r="B132">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>196</v>
+      </c>
+      <c r="B133">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>197</v>
+      </c>
+      <c r="B134">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>198</v>
+      </c>
+      <c r="B135">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>199</v>
+      </c>
+      <c r="B136">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>200</v>
+      </c>
+      <c r="B137">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>201</v>
+      </c>
+      <c r="B138">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>202</v>
+      </c>
+      <c r="B139">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>203</v>
+      </c>
+      <c r="B140">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>204</v>
+      </c>
+      <c r="B141">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>205</v>
+      </c>
+      <c r="B142">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>206</v>
+      </c>
+      <c r="B143">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>207</v>
+      </c>
+      <c r="B144">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>208</v>
+      </c>
+      <c r="B145">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>209</v>
+      </c>
+      <c r="B146">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>210</v>
+      </c>
+      <c r="B147">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>211</v>
+      </c>
+      <c r="B148">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>212</v>
+      </c>
+      <c r="B149">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>213</v>
+      </c>
+      <c r="B150">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>214</v>
+      </c>
+      <c r="B151">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>215</v>
+      </c>
+      <c r="B152">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>216</v>
+      </c>
+      <c r="B153">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>217</v>
+      </c>
+      <c r="B154">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>218</v>
+      </c>
+      <c r="B155">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>219</v>
+      </c>
+      <c r="B156">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>220</v>
+      </c>
+      <c r="B157">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>221</v>
+      </c>
+      <c r="B158">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>222</v>
+      </c>
+      <c r="B159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>223</v>
+      </c>
+      <c r="B160">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>224</v>
+      </c>
+      <c r="B161">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>225</v>
+      </c>
+      <c r="B162">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>226</v>
+      </c>
+      <c r="B163">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>227</v>
+      </c>
+      <c r="B164">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>228</v>
+      </c>
+      <c r="B165">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>229</v>
+      </c>
+      <c r="B166">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>230</v>
+      </c>
+      <c r="B167">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>231</v>
+      </c>
+      <c r="B168">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>232</v>
+      </c>
+      <c r="B169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>233</v>
+      </c>
+      <c r="B170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>234</v>
+      </c>
+      <c r="B171">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>235</v>
+      </c>
+      <c r="B172">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>236</v>
+      </c>
+      <c r="B173">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>237</v>
+      </c>
+      <c r="B174">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>238</v>
+      </c>
+      <c r="B175">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>239</v>
+      </c>
+      <c r="B176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>240</v>
+      </c>
+      <c r="B177">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>241</v>
+      </c>
+      <c r="B178">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>242</v>
+      </c>
+      <c r="B179">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>243</v>
+      </c>
+      <c r="B180">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>244</v>
+      </c>
+      <c r="B181">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>5</v>
+      </c>
+      <c r="B182">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>6</v>
+      </c>
+      <c r="B183">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>7</v>
+      </c>
+      <c r="B184">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>8</v>
+      </c>
+      <c r="B185">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>9</v>
+      </c>
+      <c r="B186">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>10</v>
+      </c>
+      <c r="B187">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>11</v>
+      </c>
+      <c r="B188">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>12</v>
+      </c>
+      <c r="B189">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>13</v>
+      </c>
+      <c r="B190">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>14</v>
+      </c>
+      <c r="B191">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>15</v>
+      </c>
+      <c r="B192">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>16</v>
+      </c>
+      <c r="B193">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>17</v>
+      </c>
+      <c r="B194">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>18</v>
+      </c>
+      <c r="B195">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>19</v>
+      </c>
+      <c r="B196">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>20</v>
+      </c>
+      <c r="B197">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>21</v>
+      </c>
+      <c r="B198">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>22</v>
+      </c>
+      <c r="B199">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>23</v>
+      </c>
+      <c r="B200">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>24</v>
+      </c>
+      <c r="B201">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>25</v>
+      </c>
+      <c r="B202">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>26</v>
+      </c>
+      <c r="B203">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>27</v>
+      </c>
+      <c r="B204">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>28</v>
+      </c>
+      <c r="B205">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>29</v>
+      </c>
+      <c r="B206">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>30</v>
+      </c>
+      <c r="B207">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>31</v>
+      </c>
+      <c r="B208">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>32</v>
+      </c>
+      <c r="B209">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>33</v>
+      </c>
+      <c r="B210">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>34</v>
+      </c>
+      <c r="B211">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>35</v>
+      </c>
+      <c r="B212">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>36</v>
+      </c>
+      <c r="B213">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>37</v>
+      </c>
+      <c r="B214">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>38</v>
+      </c>
+      <c r="B215">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>39</v>
+      </c>
+      <c r="B216">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>40</v>
+      </c>
+      <c r="B217">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>41</v>
+      </c>
+      <c r="B218">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>42</v>
+      </c>
+      <c r="B219">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>43</v>
+      </c>
+      <c r="B220">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>44</v>
+      </c>
+      <c r="B221">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>45</v>
+      </c>
+      <c r="B222">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>46</v>
+      </c>
+      <c r="B223">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>47</v>
+      </c>
+      <c r="B224">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>48</v>
+      </c>
+      <c r="B225">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>49</v>
+      </c>
+      <c r="B226">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>50</v>
+      </c>
+      <c r="B227">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>51</v>
+      </c>
+      <c r="B228">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>52</v>
       </c>
-      <c r="B49">
+      <c r="B229">
         <v>2.8</v>
       </c>
     </row>

</xml_diff>